<commit_message>
Downloading a file in browser
</commit_message>
<xml_diff>
--- a/data/data-selectedUnvi.xlsx
+++ b/data/data-selectedUnvi.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>지원 가능 대학</t>
   </si>
@@ -164,7 +164,7 @@
     <t>2019전형평균</t>
   </si>
   <si>
-    <t>동국대</t>
+    <t>고려대</t>
   </si>
   <si>
     <t>수시</t>
@@ -173,19 +173,19 @@
     <t>학생부교과</t>
   </si>
   <si>
-    <t>학교장추천인재</t>
-  </si>
-  <si>
-    <t>멀티미디어공학과</t>
+    <t>학교추천</t>
+  </si>
+  <si>
+    <t>건축학과</t>
   </si>
   <si>
     <t>자연</t>
   </si>
   <si>
-    <t>미디어</t>
-  </si>
-  <si>
-    <t>국내 고교 졸업(예정)자로서 소속 고등학교장의 추천을 받은 자, 고교별 추천인원 7명 이내(인문계열 4명 이내, 자연계열 4명 이내)</t>
+    <t>건축공</t>
+  </si>
+  <si>
+    <t>국내 고교 졸업(예정)자로서 출신 고등학교 추천을 받은 자, 고교별 재적 학생 수의 4%까지 추천, 계열별 지원인원 제한 없음, 특성화고 및 일반고 등 전문계 과정은 지원 불가</t>
   </si>
   <si>
     <t>일괄합산</t>
@@ -194,109 +194,271 @@
     <t/>
   </si>
   <si>
-    <t>교과(60) + 서류(40)</t>
+    <t>교과(80) + 서류(20)</t>
+  </si>
+  <si>
+    <t>국어, 수학(미적분/기하), 영어, 과탐(2과목 평균) 중 3개 합 6등급 이내 및 한국사 4등급 이내</t>
+  </si>
+  <si>
+    <t>교과 80, 가중치 없음, 국수영사과한국사 교과 중 상위 12과목, 과학 2과목 필수, 석차등급</t>
+  </si>
+  <si>
+    <t>학업역량, 자기계발역량(70), 인성(30), 과제해결능력</t>
+  </si>
+  <si>
+    <t>해당없음</t>
+  </si>
+  <si>
+    <t>학교생활기록부</t>
+  </si>
+  <si>
+    <t>{ false}</t>
+  </si>
+  <si>
+    <t>2022부터 자소서 폐지</t>
+  </si>
+  <si>
+    <t>9.10.(금) ~ 9.13.(월) 17:00</t>
+  </si>
+  <si>
+    <t>12.16.(목) 17:00</t>
+  </si>
+  <si>
+    <t>4.69:1</t>
+  </si>
+  <si>
+    <t>4.58:1</t>
+  </si>
+  <si>
+    <t>7.08:1</t>
+  </si>
+  <si>
+    <t>수원대</t>
+  </si>
+  <si>
+    <t>교과논술</t>
+  </si>
+  <si>
+    <t>건축도시부동산학부</t>
+  </si>
+  <si>
+    <t>고교 졸업(예정)자 또는 검정고시 합격자</t>
+  </si>
+  <si>
+    <t>논술(60) + 교과(40)</t>
   </si>
   <si>
     <t>없음</t>
   </si>
   <si>
-    <t>교과 60, 국수영과 각 교과별 상위 5과목, 점수가 높은 순으로 30:30:25:15, 석차등급</t>
-  </si>
-  <si>
-    <t>제출서류기반 지원동기(10) 자기주도적 학습능력(40) 전공적합성(30) 인성 및 사회성(20)</t>
-  </si>
-  <si>
-    <t>해당없음</t>
-  </si>
-  <si>
-    <t>학교생활기록부</t>
-  </si>
-  <si>
-    <t>{ false}</t>
+    <t>교과 40, 가중치 없음, 국수영통사통과사회, 석차등급</t>
+  </si>
+  <si>
+    <t>2022 신설</t>
+  </si>
+  <si>
+    <t>9.10.(금) ~ 9.14.(화) 18:00</t>
+  </si>
+  <si>
+    <t>(논술)11.19.(금) ~ 11.22.(월)</t>
+  </si>
+  <si>
+    <t>12.16.(목) 17:00 이전</t>
+  </si>
+  <si>
+    <t>6.28:1</t>
+  </si>
+  <si>
+    <t>8.88:1</t>
+  </si>
+  <si>
+    <t>10.60:1</t>
+  </si>
+  <si>
+    <t>교과우수</t>
+  </si>
+  <si>
+    <t>2017년 2월 이후 국내 고교 졸업(예정)자</t>
+  </si>
+  <si>
+    <t>교과(100)</t>
+  </si>
+  <si>
+    <t>국어, 수학, 영어, 탐구(1과목) 중 1개 영역 4등급 이내</t>
+  </si>
+  <si>
+    <t>교과 100, 국수영과 각 교과별 상위 5과목, 점수가 높은 순으로 30:30:25:15, 석차등급</t>
+  </si>
+  <si>
+    <t>2022 학생부교과 100% 명칭 변경</t>
+  </si>
+  <si>
+    <t>6.60:1</t>
+  </si>
+  <si>
+    <t>6.00:1</t>
+  </si>
+  <si>
+    <t>12.10:1</t>
+  </si>
+  <si>
+    <t>면접(위주)교과</t>
+  </si>
+  <si>
+    <t>단계별</t>
+  </si>
+  <si>
+    <t>5배수</t>
+  </si>
+  <si>
+    <t>1단계(60) + 면접(40)</t>
+  </si>
+  <si>
+    <t>교과 60, 가중치 없음, 국수영사과 교과 중 상위 12과목, 석차등급</t>
+  </si>
+  <si>
+    <t>그룹면접(3명) 구술면접, 자기소개(1분), 인성, 창의력 및 사고력, 전공 적합성, 학업계획 및 포부</t>
+  </si>
+  <si>
+    <t>2022 미래인재면접전형 명칭변경</t>
+  </si>
+  <si>
+    <t>9.28.(화)</t>
+  </si>
+  <si>
+    <t>(면접)10.07.(목) ~ 10.10.(일)</t>
+  </si>
+  <si>
+    <t>11.12.(금) 17:00 이전</t>
+  </si>
+  <si>
+    <t>6.15:1</t>
+  </si>
+  <si>
+    <t>7.50:1</t>
+  </si>
+  <si>
+    <t>8.95:1</t>
+  </si>
+  <si>
+    <t>지역균형선발</t>
+  </si>
+  <si>
+    <t>2017년 2월 이후 국내 고교 졸업(예정)자로서 소속 학교장 추천을 받은 자, 고교별 3학년 입학정원의 10%이내</t>
+  </si>
+  <si>
+    <t>교과(60) + 면접(40)</t>
+  </si>
+  <si>
+    <t>(면접)11.24.(수) ~ 11.28.(일)</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>아주대</t>
+  </si>
+  <si>
+    <t>고교추천</t>
+  </si>
+  <si>
+    <t>2020년 1월 이후 국내 고교 졸업(예정)자로서 3학년 1학기까지 전 학기를 모두 이수한 자</t>
+  </si>
+  <si>
+    <t>국어, 수학, 영어, 과탐(1과목) 중 2개 합 4등급 이내</t>
+  </si>
+  <si>
+    <t>교과 100, 1학년(20) 2~3학년(80), 국(20)수(30)영(30)과(20) 교과 전과목, 석차등급</t>
+  </si>
+  <si>
+    <t>2022 학업우수자 명칭 변경</t>
   </si>
   <si>
     <t>9.10.(금) ~ 9.14.(화) 17:00</t>
   </si>
   <si>
-    <t>11.26.(금)</t>
-  </si>
-  <si>
-    <t>5.6:1</t>
-  </si>
-  <si>
-    <t>3.0:1</t>
-  </si>
-  <si>
-    <t>6.0:1</t>
-  </si>
-  <si>
-    <t>서울여대</t>
-  </si>
-  <si>
-    <t>교과우수자</t>
-  </si>
-  <si>
-    <t>디지털미디어학과</t>
-  </si>
-  <si>
-    <t>고교 졸업(예정)자 중 국내 고교 전 교육과정을 이수한 자로서 학교장 추천을 받은 자, 고교별 추천인원 제한 없음</t>
-  </si>
-  <si>
-    <t>교과(100)</t>
-  </si>
-  <si>
-    <t>국어, 수학, 영어, 탐구(1과목) 중 2개 합 7등급 이내(단, 영어포함시 2개 합 5등급 이내)</t>
-  </si>
-  <si>
-    <t>교과 100, 가중치 없음, 국수영사/과 교과별 상위 3과목씩 총 12과목, 석차등급</t>
-  </si>
-  <si>
-    <t>9.10.(금) ~ 9.14.(화) 18:00</t>
-  </si>
-  <si>
     <t>12.16.(목)</t>
   </si>
   <si>
-    <t>5.2:1</t>
-  </si>
-  <si>
-    <t>6.9:1</t>
-  </si>
-  <si>
-    <t>12.9:1</t>
-  </si>
-  <si>
-    <t>숭실대</t>
-  </si>
-  <si>
-    <t>학생부우수자-학교장추천</t>
-  </si>
-  <si>
-    <t>글로벌미디어학부</t>
-  </si>
-  <si>
-    <t>2022년 2월 졸업예정자, 3학기 이상 이수하고 학생부 교과성적이 산출 가능한 출신 고등학교의 추천을 받은 자</t>
-  </si>
-  <si>
-    <t>국어, 수학(미적분/기하), 과탐(2과목 평균) 2개 합 7등급 이내</t>
-  </si>
-  <si>
-    <t>교과 100, (공통/일반선택)국(15)수(35)영(25)과(25) 전과목, 석차등급 (진로선택)성취도 등급</t>
-  </si>
-  <si>
-    <t>9.11.(토) ~ 9.14.(화) 18:00</t>
-  </si>
-  <si>
-    <t>70%컷</t>
-  </si>
-  <si>
-    <t>4.65:1</t>
-  </si>
-  <si>
-    <t>6.24:1</t>
-  </si>
-  <si>
-    <t>7.59:1</t>
+    <t>4.8:1</t>
+  </si>
+  <si>
+    <t>4.80:1</t>
+  </si>
+  <si>
+    <t>4.33:1</t>
+  </si>
+  <si>
+    <t>중앙대</t>
+  </si>
+  <si>
+    <t>지역균형</t>
+  </si>
+  <si>
+    <t>건설환경플랜트공학</t>
+  </si>
+  <si>
+    <t>국내 고교 졸업(예정)자로서 3학기 이상 성적을 취득한 자이며 소속 고등학교장의 추천을 받은 자</t>
+  </si>
+  <si>
+    <t>교과(70) + 출결 및 봉사(30)</t>
+  </si>
+  <si>
+    <t>국어, 수학(미적분/기하), 영어, 과탐(2과목 평균) 중 3개 합 7등급 이내 및 한국사 4등급 이내</t>
+  </si>
+  <si>
+    <t>교과 70, 가중치 없음, (공통/일반선택)국수영 중 2개 교과 + 사과 중 1개 교과, 합 3개교과, 석차등급, (진로선택)3개 과목, 성취도</t>
+  </si>
+  <si>
+    <t>(출결)무단/미인정 1일 이하, (봉사)전원 만점 처리</t>
+  </si>
+  <si>
+    <t>2022학년도 학생부교과전형에서 개명</t>
+  </si>
+  <si>
+    <t>12.16.(목) 14:00</t>
+  </si>
+  <si>
+    <t>14.38:1</t>
+  </si>
+  <si>
+    <t>14.20:1</t>
+  </si>
+  <si>
+    <t>25.00:1</t>
+  </si>
+  <si>
+    <t>충북대</t>
+  </si>
+  <si>
+    <t>지역인재</t>
+  </si>
+  <si>
+    <t>국내 고교 졸업(예정)자 중 충청권소재 고교 전교육과정 이수자</t>
+  </si>
+  <si>
+    <t>국어, 수학, 영어, 과탐(2과목 평균) 중 3개 합 13등급 이내</t>
+  </si>
+  <si>
+    <t>교과 100, 가중치 없음, (고1)국수영사과, (고2·3)국영수과, 석차등급</t>
+  </si>
+  <si>
+    <t>9.10.(금) ~ 9.14.(화) 19:00</t>
+  </si>
+  <si>
+    <t>12.16.(목) 17:00 (예정)</t>
+  </si>
+  <si>
+    <t>9.00:1</t>
+  </si>
+  <si>
+    <t>국내 고교 졸업(예정)자 또는 동등이상 학력 인정된 자, ※국내 고등학교 학교생활기록부가 없는 자는 지원 불가능</t>
+  </si>
+  <si>
+    <t>국어, 수학, 영어, 과탐(2과목 평균) 중 3개 합 12등급 이내</t>
+  </si>
+  <si>
+    <t>7.60:1</t>
   </si>
 </sst>
 </file>
@@ -806,7 +968,7 @@
         <v>55</v>
       </c>
       <c r="I3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J3" t="s">
         <v>56</v>
@@ -848,10 +1010,10 @@
         <v>65</v>
       </c>
       <c r="W3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="X3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Y3" t="s">
         <v>58</v>
@@ -863,58 +1025,58 @@
         <v>58</v>
       </c>
       <c r="AB3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AC3" t="s">
         <v>58</v>
       </c>
       <c r="AD3">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="AE3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AF3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG3">
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>2.28</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <v>2.71</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
         <v>0</v>
       </c>
       <c r="AK3">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="AL3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AM3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN3">
         <v>0</v>
       </c>
       <c r="AO3">
-        <v>2.82</v>
+        <v>0</v>
       </c>
       <c r="AP3">
-        <v>4.02</v>
+        <v>0</v>
       </c>
       <c r="AQ3">
         <v>0</v>
       </c>
       <c r="AR3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AS3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AT3">
         <v>0</v>
@@ -923,10 +1085,10 @@
         <v>0</v>
       </c>
       <c r="AV3">
-        <v>1.96</v>
+        <v>0</v>
       </c>
       <c r="AW3">
-        <v>2.45</v>
+        <v>0</v>
       </c>
       <c r="AX3">
         <v>0</v>
@@ -937,7 +1099,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
         <v>50</v>
@@ -946,10 +1108,10 @@
         <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G4" t="s">
         <v>54</v>
@@ -958,10 +1120,10 @@
         <v>55</v>
       </c>
       <c r="I4">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K4" t="s">
         <v>57</v>
@@ -973,13 +1135,13 @@
         <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Q4" t="s">
         <v>63</v>
@@ -988,7 +1150,7 @@
         <v>63</v>
       </c>
       <c r="S4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="T4" t="s">
         <v>63</v>
@@ -1000,10 +1162,10 @@
         <v>65</v>
       </c>
       <c r="W4" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="X4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Y4" t="s">
         <v>58</v>
@@ -1012,61 +1174,61 @@
         <v>58</v>
       </c>
       <c r="AA4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="AB4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="AC4" t="s">
         <v>58</v>
       </c>
       <c r="AD4">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="AE4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AF4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AG4">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="AH4">
-        <v>2.5</v>
+        <v>4.4</v>
       </c>
       <c r="AI4">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="AJ4">
         <v>0</v>
       </c>
       <c r="AK4">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="AL4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AM4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AN4">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="AO4">
-        <v>1.9</v>
+        <v>5.1</v>
       </c>
       <c r="AP4">
-        <v>2.4</v>
+        <v>6.3</v>
       </c>
       <c r="AQ4">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AR4">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="AS4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AT4">
         <v>0</v>
@@ -1075,13 +1237,13 @@
         <v>0</v>
       </c>
       <c r="AV4">
-        <v>2</v>
+        <v>4.9</v>
       </c>
       <c r="AW4">
-        <v>2.2</v>
+        <v>0</v>
       </c>
       <c r="AX4">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
@@ -1089,7 +1251,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
         <v>50</v>
@@ -1098,10 +1260,10 @@
         <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
         <v>54</v>
@@ -1110,10 +1272,10 @@
         <v>55</v>
       </c>
       <c r="I5">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K5" t="s">
         <v>57</v>
@@ -1125,13 +1287,13 @@
         <v>58</v>
       </c>
       <c r="N5" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="P5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="Q5" t="s">
         <v>63</v>
@@ -1140,7 +1302,7 @@
         <v>63</v>
       </c>
       <c r="S5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="T5" t="s">
         <v>63</v>
@@ -1152,90 +1314,1005 @@
         <v>65</v>
       </c>
       <c r="W5" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="X5" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5">
+        <v>10</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>4</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>10</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>3.5</v>
+      </c>
+      <c r="AP5">
+        <v>4.8</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>10</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>3</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" t="s">
+        <v>96</v>
+      </c>
+      <c r="L6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M6" t="s">
+        <v>97</v>
+      </c>
+      <c r="N6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" t="s">
+        <v>100</v>
+      </c>
+      <c r="S6" t="s">
+        <v>99</v>
+      </c>
+      <c r="T6" t="s">
+        <v>63</v>
+      </c>
+      <c r="U6" t="s">
+        <v>64</v>
+      </c>
+      <c r="V6" t="s">
+        <v>65</v>
+      </c>
+      <c r="W6" t="s">
+        <v>101</v>
+      </c>
+      <c r="X6" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD6">
+        <v>20</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>4</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>20</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>4.2</v>
+      </c>
+      <c r="AP6">
+        <v>4.8</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>20</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>4.3</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" t="s">
+        <v>110</v>
+      </c>
+      <c r="O7" t="s">
         <v>89</v>
       </c>
-      <c r="Y5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB5" t="s">
+      <c r="P7" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" t="s">
+        <v>100</v>
+      </c>
+      <c r="S7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U7" t="s">
+        <v>64</v>
+      </c>
+      <c r="V7" t="s">
+        <v>65</v>
+      </c>
+      <c r="W7" t="s">
         <v>79</v>
       </c>
-      <c r="AC5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD5">
-        <v>17</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF5">
-        <v>14</v>
-      </c>
-      <c r="AG5">
-        <v>0</v>
-      </c>
-      <c r="AH5">
-        <v>2.4</v>
-      </c>
-      <c r="AI5">
-        <v>3.2</v>
-      </c>
-      <c r="AJ5">
-        <v>0</v>
-      </c>
-      <c r="AK5">
-        <v>17</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM5">
-        <v>18</v>
-      </c>
-      <c r="AN5">
-        <v>0</v>
-      </c>
-      <c r="AO5">
-        <v>2.3</v>
-      </c>
-      <c r="AP5">
-        <v>2.3</v>
-      </c>
-      <c r="AQ5">
-        <v>0</v>
-      </c>
-      <c r="AR5">
-        <v>17</v>
-      </c>
-      <c r="AS5" t="s">
+      <c r="X7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>10</v>
+      </c>
+      <c r="AL7" t="s">
         <v>93</v>
       </c>
-      <c r="AT5">
-        <v>0</v>
-      </c>
-      <c r="AU5">
-        <v>0</v>
-      </c>
-      <c r="AV5">
-        <v>2.4</v>
-      </c>
-      <c r="AW5">
-        <v>0</v>
-      </c>
-      <c r="AX5">
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>3.5</v>
+      </c>
+      <c r="AP7">
+        <v>4.8</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>10</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>3</v>
+      </c>
+      <c r="AW7">
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+      <c r="J8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" t="s">
+        <v>88</v>
+      </c>
+      <c r="O8" t="s">
+        <v>116</v>
+      </c>
+      <c r="P8" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" t="s">
+        <v>63</v>
+      </c>
+      <c r="S8" t="s">
+        <v>117</v>
+      </c>
+      <c r="T8" t="s">
+        <v>63</v>
+      </c>
+      <c r="U8" t="s">
+        <v>64</v>
+      </c>
+      <c r="V8" t="s">
+        <v>65</v>
+      </c>
+      <c r="W8" t="s">
+        <v>118</v>
+      </c>
+      <c r="X8" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD8">
+        <v>10</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>2.45</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>10</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>1.89</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>15</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <v>1.88</v>
+      </c>
+      <c r="AW8">
+        <v>0</v>
+      </c>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>127</v>
+      </c>
+      <c r="K9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9" t="s">
+        <v>128</v>
+      </c>
+      <c r="O9" t="s">
+        <v>129</v>
+      </c>
+      <c r="P9" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" t="s">
+        <v>63</v>
+      </c>
+      <c r="S9" t="s">
+        <v>130</v>
+      </c>
+      <c r="T9" t="s">
+        <v>131</v>
+      </c>
+      <c r="U9" t="s">
+        <v>64</v>
+      </c>
+      <c r="V9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W9" t="s">
+        <v>132</v>
+      </c>
+      <c r="X9" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD9">
+        <v>8</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF9">
+        <v>12</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>1.7</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>5</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>1.8</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>7</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9">
+        <v>1.86</v>
+      </c>
+      <c r="AW9">
+        <v>0</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10" t="s">
+        <v>139</v>
+      </c>
+      <c r="K10" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" t="s">
+        <v>88</v>
+      </c>
+      <c r="O10" t="s">
+        <v>140</v>
+      </c>
+      <c r="P10" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>63</v>
+      </c>
+      <c r="R10" t="s">
+        <v>63</v>
+      </c>
+      <c r="S10" t="s">
+        <v>141</v>
+      </c>
+      <c r="T10" t="s">
+        <v>63</v>
+      </c>
+      <c r="U10" t="s">
+        <v>64</v>
+      </c>
+      <c r="V10" t="s">
+        <v>65</v>
+      </c>
+      <c r="W10" t="s">
+        <v>58</v>
+      </c>
+      <c r="X10" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>3</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>144</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>3.14</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>75.73</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>0</v>
+      </c>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="J11" t="s">
+        <v>145</v>
+      </c>
+      <c r="K11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" t="s">
+        <v>58</v>
+      </c>
+      <c r="N11" t="s">
+        <v>88</v>
+      </c>
+      <c r="O11" t="s">
+        <v>146</v>
+      </c>
+      <c r="P11" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>63</v>
+      </c>
+      <c r="R11" t="s">
+        <v>63</v>
+      </c>
+      <c r="S11" t="s">
+        <v>141</v>
+      </c>
+      <c r="T11" t="s">
+        <v>63</v>
+      </c>
+      <c r="U11" t="s">
+        <v>64</v>
+      </c>
+      <c r="V11" t="s">
+        <v>65</v>
+      </c>
+      <c r="W11" t="s">
+        <v>58</v>
+      </c>
+      <c r="X11" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>10</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>147</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>3.29</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11">
+        <v>75.42</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11">
+        <v>0</v>
+      </c>
+      <c r="AX11">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:T1"/>
+  </mergeCells>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
first commit of cnest_consult
</commit_message>
<xml_diff>
--- a/data/data-selectedUnvi.xlsx
+++ b/data/data-selectedUnvi.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
   <si>
     <t>지원 가능 대학</t>
   </si>
@@ -164,67 +164,352 @@
     <t>2019전형평균</t>
   </si>
   <si>
-    <t>인하대</t>
+    <t>명지대</t>
   </si>
   <si>
     <t>수시</t>
   </si>
   <si>
-    <t>학생부교과</t>
-  </si>
-  <si>
-    <t>지역추천인재</t>
-  </si>
-  <si>
-    <t>컴퓨터공학과</t>
-  </si>
-  <si>
-    <t>공통</t>
+    <t>학생부종합</t>
+  </si>
+  <si>
+    <t>명지인재면접</t>
+  </si>
+  <si>
+    <t>교통공학과</t>
+  </si>
+  <si>
+    <t>자연</t>
   </si>
   <si>
     <t>공학기타</t>
   </si>
   <si>
-    <t>국내 고교에서 3학기 이상 이수한 졸업(예정)자로서 소속(졸업) 고등학교장의 추천을 받은 자, 고교별 7명 이내</t>
+    <t>고교 졸업(예정)자 / 동등학력 이상 / 국내 학생부 3학기 이상</t>
+  </si>
+  <si>
+    <t>단계별</t>
+  </si>
+  <si>
+    <t>서류(100)</t>
+  </si>
+  <si>
+    <t>3배수</t>
+  </si>
+  <si>
+    <t>1단계(70) + 면접(30)</t>
+  </si>
+  <si>
+    <t>없음</t>
+  </si>
+  <si>
+    <t>교과 95, 가중치 없음, 국영사/수영과 중 학기당 교과별 1과목, 총 15과목, 석차등급</t>
+  </si>
+  <si>
+    <t>인성(20) 학업역량(20) 전공적성(30) 발전가능성(30)</t>
+  </si>
+  <si>
+    <t>1:2 제출서류기반 개별면접, 인성(30) 전공적합성(40) 의사소통능력(30), 10분내외</t>
+  </si>
+  <si>
+    <t>해당없음</t>
+  </si>
+  <si>
+    <t>학교생활기록부</t>
+  </si>
+  <si>
+    <t>{ false}</t>
+  </si>
+  <si>
+    <t>2022 명지인재에서 분리</t>
+  </si>
+  <si>
+    <t>9.10.(금) ~ 9.14.(화) 18:00</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>11.19.(금) 15:00</t>
+  </si>
+  <si>
+    <t>11.28.(일)</t>
+  </si>
+  <si>
+    <t>12.9.(목) 15:00</t>
+  </si>
+  <si>
+    <t>4.2:1</t>
+  </si>
+  <si>
+    <t>4.18:1</t>
+  </si>
+  <si>
+    <t>7.8:1</t>
+  </si>
+  <si>
+    <t>명지인재서류</t>
   </si>
   <si>
     <t>일괄합산</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>교과(100)</t>
-  </si>
-  <si>
-    <t>국어, 수학, 영어, 탐구(1과목) 중 2개 합 5등급 이내</t>
-  </si>
-  <si>
-    <t>교과 100, 가중치 없음, 국수영사 전과목, 석차등급</t>
-  </si>
-  <si>
-    <t>해당없음</t>
-  </si>
-  <si>
-    <t>학교생활기록부</t>
-  </si>
-  <si>
-    <t>{ false}</t>
-  </si>
-  <si>
-    <t>2022 신설</t>
-  </si>
-  <si>
-    <t>9.10.(금) ~ 9.14.(화) 18:00</t>
+    <t>인성(20) 학업역량(30) 전공적성(30) 발전가능성(20)</t>
+  </si>
+  <si>
+    <t>학교생활기록부, 자기소개서</t>
+  </si>
+  <si>
+    <t>{없음 true}</t>
+  </si>
+  <si>
+    <t>서울시립대</t>
+  </si>
+  <si>
+    <t>고교 졸업(예정)자 또는 동등학력 이상 인정된 자</t>
+  </si>
+  <si>
+    <t>2~4배수</t>
+  </si>
+  <si>
+    <t>1단계(60) + 면접(40)</t>
+  </si>
+  <si>
+    <t>학업역량(35) 잠재역량(40) 사회역량(25)</t>
+  </si>
+  <si>
+    <t>1:2 제출서류기반 개별면접, 학업역량(35) 잠재역량(40) 사회역량(25), 15분</t>
+  </si>
+  <si>
+    <t>{지원동기 및 진로계획 800자 true}</t>
+  </si>
+  <si>
+    <t>9.10.(금) ~ 9.13.(월) 18:00</t>
+  </si>
+  <si>
+    <t>9.14.(화) 18:00</t>
+  </si>
+  <si>
+    <t>11.19.(금)</t>
+  </si>
+  <si>
+    <t>(면접)11.27.(토)</t>
   </si>
   <si>
     <t>12.16.(목)</t>
   </si>
   <si>
-    <t>6.7:1</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>5.88:1</t>
+  </si>
+  <si>
+    <t>6.25:1</t>
+  </si>
+  <si>
+    <t>6.13:1</t>
+  </si>
+  <si>
+    <t>성균관대</t>
+  </si>
+  <si>
+    <t>계열모집</t>
+  </si>
+  <si>
+    <t>공학계열</t>
+  </si>
+  <si>
+    <t>학업수월성(25) 학업충실성(25) 전공적합성(15) 활동다양성(15) 자기주도성(10) 발전가능성(10)</t>
+  </si>
+  <si>
+    <t>{지원동기 및 노력 800자 true}</t>
+  </si>
+  <si>
+    <t>2020부터 성균인재전형에서 명칭변경모집</t>
+  </si>
+  <si>
+    <t>9.10.(금) ~ 9.13.(월) 17:00</t>
+  </si>
+  <si>
+    <t>9.14.(화) 17:00</t>
+  </si>
+  <si>
+    <t>12.16.(목) 이전</t>
+  </si>
+  <si>
+    <t>11.56:1</t>
+  </si>
+  <si>
+    <t>13.78:1</t>
+  </si>
+  <si>
+    <t>8.35:1</t>
+  </si>
+  <si>
+    <t>세종대</t>
+  </si>
+  <si>
+    <t>창의인재</t>
+  </si>
+  <si>
+    <t>디자인이노베이션전공</t>
+  </si>
+  <si>
+    <t>학업역량(30) 전공적합성(35) 창의성 및 발전가능성(20) 인성(15)</t>
+  </si>
+  <si>
+    <t>1:2 제출서류기반 개별면접, 전공적합성(40) 발전가능성(35) 의사소통능력 및 인성(25), 9분 내외</t>
+  </si>
+  <si>
+    <t>9.15.(수) 17:00</t>
+  </si>
+  <si>
+    <t>11.25.(목)</t>
+  </si>
+  <si>
+    <t>(면접)12.04.(토)</t>
+  </si>
+  <si>
+    <t>12.16.(목) 17:00 이후</t>
+  </si>
+  <si>
+    <t>70%컷</t>
+  </si>
+  <si>
+    <t>8.23:1</t>
+  </si>
+  <si>
+    <t>7.90:1</t>
+  </si>
+  <si>
+    <t>9.71:1</t>
+  </si>
+  <si>
+    <t>아주대</t>
+  </si>
+  <si>
+    <t>ACE</t>
+  </si>
+  <si>
+    <t>교통시스템공학과</t>
+  </si>
+  <si>
+    <t>학업역량(28) 목표의식(17) 자기주도성(20) 공동체의식(15) 성실성(20)</t>
+  </si>
+  <si>
+    <t>1:2 제출서류기반 개별면접, 학업역량(36) 주도성(34) 대인역량(20) 의사소통능력(10), 10분 내외</t>
+  </si>
+  <si>
+    <t>{지원동기와 학업계획 800자 true}</t>
+  </si>
+  <si>
+    <t>9.10.(금) ~ 9.14.(화) 17:00</t>
+  </si>
+  <si>
+    <t>9.24.(금) 17:00</t>
+  </si>
+  <si>
+    <t>11.16.(화)</t>
+  </si>
+  <si>
+    <t>11.21.(일)</t>
+  </si>
+  <si>
+    <t>5.2:1</t>
+  </si>
+  <si>
+    <t>5.62:1</t>
+  </si>
+  <si>
+    <t>7.07:1</t>
+  </si>
+  <si>
+    <t>미디어학과</t>
+  </si>
+  <si>
+    <t>7.98:1</t>
+  </si>
+  <si>
+    <t>7.11:1</t>
+  </si>
+  <si>
+    <t>8.04:1</t>
+  </si>
+  <si>
+    <t>다산인재</t>
+  </si>
+  <si>
+    <t>고교 졸업(예정)자 또는 동등학력 이상 인정된 자로서 다산형 인재 핵심역량(융복합 사고 역량, 실천적 창의 역량, 의사소통 역량, 글로벌 역량)에 강점이 있는 자</t>
+  </si>
+  <si>
+    <t>학업역량(30) 목표의식(20) 자기주도성(31) 공동체의식(9) 성실성(10)</t>
+  </si>
+  <si>
+    <t>5.0:1</t>
+  </si>
+  <si>
+    <t>5.25:1</t>
+  </si>
+  <si>
+    <t>5.57:1</t>
+  </si>
+  <si>
+    <t>7.38:1</t>
+  </si>
+  <si>
+    <t>10.081:1</t>
+  </si>
+  <si>
+    <t>7.50:1</t>
+  </si>
+  <si>
+    <t>한국기술교대</t>
+  </si>
+  <si>
+    <t>지역인재</t>
+  </si>
+  <si>
+    <t>디자인공학전공</t>
+  </si>
+  <si>
+    <t>고교 졸업(예정)자로서 대전-세종-충남-충북지역 소재 정규 고교에서 입학부터 졸업까지 3학년 전 과정을 이수한 자</t>
+  </si>
+  <si>
+    <t>4배수</t>
+  </si>
+  <si>
+    <t>학업역량(20), 전공적합성(20), 나우리인성(20), 발전가능성(40)</t>
+  </si>
+  <si>
+    <t>1:1 제출서류기반 개별면접, 전공적합성영역(10분 내외), 인성영역(10분 내외)</t>
+  </si>
+  <si>
+    <t>9.10.(금) ~ 9.14.(화) 19:00</t>
+  </si>
+  <si>
+    <t>11.03.(수) (예정)</t>
+  </si>
+  <si>
+    <t>(면접)11.07.(일)</t>
+  </si>
+  <si>
+    <t>11.19.(금) (예정)</t>
+  </si>
+  <si>
+    <t>5.33:1</t>
+  </si>
+  <si>
+    <t>8.86:1</t>
+  </si>
+  <si>
+    <t>12.00:1</t>
+  </si>
+  <si>
+    <t>국내 정규 고교 졸업(예정)자로서 창의적 사고와 능동적 실천능력을 갖추고 전공 분야에 대한 열정과 우수한 재능을 가진 자</t>
+  </si>
+  <si>
+    <t>(면접)11.06.(토)</t>
+  </si>
+  <si>
+    <t>4.63:1</t>
   </si>
 </sst>
 </file>
@@ -734,7 +1019,7 @@
         <v>55</v>
       </c>
       <c r="I3">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="J3" t="s">
         <v>56</v>
@@ -746,117 +1031,1637 @@
         <v>58</v>
       </c>
       <c r="M3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" t="s">
+        <v>65</v>
+      </c>
+      <c r="U3" t="s">
+        <v>66</v>
+      </c>
+      <c r="V3" t="s">
+        <v>67</v>
+      </c>
+      <c r="W3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD3">
+        <v>11</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF3">
+        <v>11</v>
+      </c>
+      <c r="AG3">
+        <v>3.68</v>
+      </c>
+      <c r="AH3">
+        <v>4.1</v>
+      </c>
+      <c r="AI3">
+        <v>4.58</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>11</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>4.03</v>
+      </c>
+      <c r="AP3">
+        <v>4.85</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>10</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>3.88</v>
+      </c>
+      <c r="AW3">
+        <v>4.56</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" t="s">
         <v>58</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>79</v>
+      </c>
+      <c r="R4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V4" t="s">
+        <v>81</v>
+      </c>
+      <c r="W4" t="s">
+        <v>68</v>
+      </c>
+      <c r="X4" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD4">
+        <v>11</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF4">
+        <v>11</v>
+      </c>
+      <c r="AG4">
+        <v>3.68</v>
+      </c>
+      <c r="AH4">
+        <v>4.1</v>
+      </c>
+      <c r="AI4">
+        <v>4.58</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>11</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>4.03</v>
+      </c>
+      <c r="AP4">
+        <v>4.85</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>10</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>3.88</v>
+      </c>
+      <c r="AW4">
+        <v>4.56</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" t="s">
+        <v>85</v>
+      </c>
+      <c r="O5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>86</v>
+      </c>
+      <c r="R5" t="s">
+        <v>87</v>
+      </c>
+      <c r="S5" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" t="s">
+        <v>80</v>
+      </c>
+      <c r="V5" t="s">
+        <v>88</v>
+      </c>
+      <c r="W5" t="s">
+        <v>70</v>
+      </c>
+      <c r="X5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD5">
+        <v>8</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>2.32</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>8</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>3.07</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>8</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>2.9</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6">
+        <v>140</v>
+      </c>
+      <c r="J6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" t="s">
+        <v>61</v>
+      </c>
+      <c r="P6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>100</v>
+      </c>
+      <c r="R6" t="s">
+        <v>65</v>
+      </c>
+      <c r="S6" t="s">
+        <v>62</v>
+      </c>
+      <c r="T6" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" t="s">
+        <v>80</v>
+      </c>
+      <c r="V6" t="s">
+        <v>101</v>
+      </c>
+      <c r="W6" t="s">
+        <v>102</v>
+      </c>
+      <c r="X6" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD6">
+        <v>230</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>223</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM6">
+        <v>728</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>267</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7">
+        <v>48</v>
+      </c>
+      <c r="J7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" t="s">
         <v>59</v>
       </c>
-      <c r="O3" t="s">
+      <c r="N7" t="s">
         <v>60</v>
       </c>
-      <c r="P3" t="s">
+      <c r="O7" t="s">
         <v>61</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="P7" t="s">
         <v>62</v>
       </c>
-      <c r="R3" t="s">
+      <c r="Q7" t="s">
+        <v>112</v>
+      </c>
+      <c r="R7" t="s">
+        <v>113</v>
+      </c>
+      <c r="S7" t="s">
         <v>62</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7" t="s">
+        <v>80</v>
+      </c>
+      <c r="V7" t="s">
+        <v>81</v>
+      </c>
+      <c r="W7" t="s">
+        <v>70</v>
+      </c>
+      <c r="X7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD7">
+        <v>48</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF7">
+        <v>30</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>2.6</v>
+      </c>
+      <c r="AI7">
+        <v>2.91</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>48</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>120</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>2.8</v>
+      </c>
+      <c r="AP7">
+        <v>3.35</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>45</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>3.18</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" t="s">
         <v>61</v>
       </c>
-      <c r="T3" t="s">
+      <c r="P8" t="s">
         <v>62</v>
       </c>
-      <c r="U3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V3" t="s">
-        <v>64</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="Q8" t="s">
+        <v>125</v>
+      </c>
+      <c r="R8" t="s">
+        <v>126</v>
+      </c>
+      <c r="S8" t="s">
+        <v>62</v>
+      </c>
+      <c r="T8" t="s">
         <v>65</v>
       </c>
-      <c r="X3" t="s">
+      <c r="U8" t="s">
+        <v>80</v>
+      </c>
+      <c r="V8" t="s">
+        <v>127</v>
+      </c>
+      <c r="W8" t="s">
+        <v>70</v>
+      </c>
+      <c r="X8" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD8">
+        <v>10</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>2.61</v>
+      </c>
+      <c r="AH8">
+        <v>3.05</v>
+      </c>
+      <c r="AI8">
+        <v>3.78</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>13</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>3.4</v>
+      </c>
+      <c r="AP8">
+        <v>6.03</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>15</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>134</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <v>3.43</v>
+      </c>
+      <c r="AW8">
+        <v>5.31</v>
+      </c>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9" t="s">
+        <v>61</v>
+      </c>
+      <c r="P9" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>125</v>
+      </c>
+      <c r="R9" t="s">
+        <v>126</v>
+      </c>
+      <c r="S9" t="s">
+        <v>62</v>
+      </c>
+      <c r="T9" t="s">
+        <v>65</v>
+      </c>
+      <c r="U9" t="s">
+        <v>80</v>
+      </c>
+      <c r="V9" t="s">
+        <v>127</v>
+      </c>
+      <c r="W9" t="s">
+        <v>70</v>
+      </c>
+      <c r="X9" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD9">
+        <v>40</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>2.33</v>
+      </c>
+      <c r="AH9">
+        <v>3.33</v>
+      </c>
+      <c r="AI9">
+        <v>6.26</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>45</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>3.18</v>
+      </c>
+      <c r="AP9">
+        <v>6.58</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>45</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9">
+        <v>3.16</v>
+      </c>
+      <c r="AW9">
+        <v>6.03</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>140</v>
+      </c>
+      <c r="K10" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" t="s">
+        <v>61</v>
+      </c>
+      <c r="P10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>141</v>
+      </c>
+      <c r="R10" t="s">
+        <v>65</v>
+      </c>
+      <c r="S10" t="s">
+        <v>62</v>
+      </c>
+      <c r="T10" t="s">
+        <v>65</v>
+      </c>
+      <c r="U10" t="s">
+        <v>80</v>
+      </c>
+      <c r="V10" t="s">
+        <v>127</v>
+      </c>
+      <c r="W10" t="s">
+        <v>70</v>
+      </c>
+      <c r="X10" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD10">
+        <v>8</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>2.76</v>
+      </c>
+      <c r="AH10">
+        <v>3.56</v>
+      </c>
+      <c r="AI10">
+        <v>4.71</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>8</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>3.4</v>
+      </c>
+      <c r="AP10">
+        <v>4.23</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>7</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>144</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>3.37</v>
+      </c>
+      <c r="AW10">
+        <v>3.97</v>
+      </c>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>140</v>
+      </c>
+      <c r="K11" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>141</v>
+      </c>
+      <c r="R11" t="s">
+        <v>65</v>
+      </c>
+      <c r="S11" t="s">
+        <v>62</v>
+      </c>
+      <c r="T11" t="s">
+        <v>65</v>
+      </c>
+      <c r="U11" t="s">
+        <v>80</v>
+      </c>
+      <c r="V11" t="s">
+        <v>127</v>
+      </c>
+      <c r="W11" t="s">
+        <v>70</v>
+      </c>
+      <c r="X11" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD11">
+        <v>16</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>145</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>2.69</v>
+      </c>
+      <c r="AH11">
+        <v>4.2</v>
+      </c>
+      <c r="AI11">
+        <v>7.48</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>16</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>3.36</v>
+      </c>
+      <c r="AP11">
+        <v>4.42</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>16</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>147</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
+        <v>3.95</v>
+      </c>
+      <c r="AW11">
+        <v>5.77</v>
+      </c>
+      <c r="AX11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" t="s">
+        <v>152</v>
+      </c>
+      <c r="N12" t="s">
+        <v>85</v>
+      </c>
+      <c r="O12" t="s">
+        <v>61</v>
+      </c>
+      <c r="P12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>153</v>
+      </c>
+      <c r="R12" t="s">
+        <v>154</v>
+      </c>
+      <c r="S12" t="s">
+        <v>62</v>
+      </c>
+      <c r="T12" t="s">
+        <v>65</v>
+      </c>
+      <c r="U12" t="s">
         <v>66</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="V12" t="s">
+        <v>67</v>
+      </c>
+      <c r="W12" t="s">
+        <v>70</v>
+      </c>
+      <c r="X12" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD12">
+        <v>3</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>159</v>
+      </c>
+      <c r="AF12">
+        <v>2</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <v>4.25</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <v>7</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>4.16</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
+      <c r="AR12">
+        <v>6</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT12">
+        <v>0</v>
+      </c>
+      <c r="AU12">
+        <v>0</v>
+      </c>
+      <c r="AV12">
+        <v>4.37</v>
+      </c>
+      <c r="AW12">
+        <v>0</v>
+      </c>
+      <c r="AX12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>162</v>
+      </c>
+      <c r="K13" t="s">
+        <v>57</v>
+      </c>
+      <c r="L13" t="s">
         <v>58</v>
       </c>
-      <c r="Z3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB3" t="s">
+      <c r="M13" t="s">
+        <v>152</v>
+      </c>
+      <c r="N13" t="s">
+        <v>85</v>
+      </c>
+      <c r="O13" t="s">
+        <v>61</v>
+      </c>
+      <c r="P13" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>153</v>
+      </c>
+      <c r="R13" t="s">
+        <v>154</v>
+      </c>
+      <c r="S13" t="s">
+        <v>62</v>
+      </c>
+      <c r="T13" t="s">
+        <v>65</v>
+      </c>
+      <c r="U13" t="s">
+        <v>66</v>
+      </c>
+      <c r="V13" t="s">
         <v>67</v>
       </c>
-      <c r="AC3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD3">
-        <v>29</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF3">
-        <v>42</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>2.16</v>
-      </c>
-      <c r="AI3">
-        <v>2.78</v>
-      </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <v>29</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
-        <v>0</v>
-      </c>
-      <c r="AO3">
-        <v>2.16</v>
-      </c>
-      <c r="AP3">
-        <v>2.78</v>
-      </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3">
-        <v>26</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT3">
-        <v>0</v>
-      </c>
-      <c r="AU3">
-        <v>0</v>
-      </c>
-      <c r="AV3">
-        <v>0</v>
-      </c>
-      <c r="AW3">
-        <v>0</v>
-      </c>
-      <c r="AX3">
+      <c r="W13" t="s">
+        <v>70</v>
+      </c>
+      <c r="X13" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD13">
+        <v>8</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>164</v>
+      </c>
+      <c r="AF13">
+        <v>3</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <v>4.6</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <v>7</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>4.16</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13">
+        <v>6</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT13">
+        <v>0</v>
+      </c>
+      <c r="AU13">
+        <v>0</v>
+      </c>
+      <c r="AV13">
+        <v>4.37</v>
+      </c>
+      <c r="AW13">
+        <v>0</v>
+      </c>
+      <c r="AX13">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first commit of univ
</commit_message>
<xml_diff>
--- a/data/data-selectedUnvi.xlsx
+++ b/data/data-selectedUnvi.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>지원 가능 대학</t>
   </si>
@@ -164,352 +164,277 @@
     <t>2019전형평균</t>
   </si>
   <si>
-    <t>명지대</t>
+    <t>강원대(춘천)</t>
   </si>
   <si>
     <t>수시</t>
   </si>
   <si>
-    <t>학생부종합</t>
-  </si>
-  <si>
-    <t>명지인재면접</t>
-  </si>
-  <si>
-    <t>교통공학과</t>
+    <t>학생부교과</t>
+  </si>
+  <si>
+    <t>일반</t>
+  </si>
+  <si>
+    <t>건축-토목-환경공학부</t>
   </si>
   <si>
     <t>자연</t>
   </si>
   <si>
-    <t>공학기타</t>
-  </si>
-  <si>
-    <t>고교 졸업(예정)자 / 동등학력 이상 / 국내 학생부 3학기 이상</t>
-  </si>
-  <si>
-    <t>단계별</t>
-  </si>
-  <si>
-    <t>서류(100)</t>
-  </si>
-  <si>
-    <t>3배수</t>
-  </si>
-  <si>
-    <t>1단계(70) + 면접(30)</t>
+    <t>건축공</t>
+  </si>
+  <si>
+    <t>고교 졸업(예정)자 또는 동등학력 인정된 자</t>
+  </si>
+  <si>
+    <t>일괄합산</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>교과(100)</t>
+  </si>
+  <si>
+    <t>국어, 수학, 영어, 과탐(1과목) 중 3개 합 12등급 이내</t>
+  </si>
+  <si>
+    <t>교과 100, 가중치 없음, 국수영사과한국사, 석차등급</t>
+  </si>
+  <si>
+    <t>해당없음</t>
+  </si>
+  <si>
+    <t>학교생활기록부</t>
+  </si>
+  <si>
+    <t>{ false}</t>
+  </si>
+  <si>
+    <t>9.10.(금) ~ 9.14.(화) 20:00</t>
+  </si>
+  <si>
+    <t>12.16.(목)</t>
+  </si>
+  <si>
+    <t>4.95:1</t>
+  </si>
+  <si>
+    <t>7.3:1</t>
+  </si>
+  <si>
+    <t>8.9:1</t>
+  </si>
+  <si>
+    <t>지역인재</t>
+  </si>
+  <si>
+    <t>고교 졸업(예정)자로서 학생이 입학일부터 졸업(예정)일까지 강원지역 고교에서 전 교육과정을 이수한 자</t>
+  </si>
+  <si>
+    <t>3.29:1</t>
+  </si>
+  <si>
+    <t>5.2:1</t>
+  </si>
+  <si>
+    <t>3.5:1</t>
+  </si>
+  <si>
+    <t>동국대</t>
+  </si>
+  <si>
+    <t>학교장추천인재</t>
+  </si>
+  <si>
+    <t>건설환경공학과</t>
+  </si>
+  <si>
+    <t>국내 고교 졸업(예정)자로서 소속 고등학교장의 추천을 받은 자, 고교별 추천인원 7명 이내(인문계열 4명 이내, 자연계열 4명 이내)</t>
+  </si>
+  <si>
+    <t>교과(60) + 서류(40)</t>
   </si>
   <si>
     <t>없음</t>
   </si>
   <si>
-    <t>교과 95, 가중치 없음, 국영사/수영과 중 학기당 교과별 1과목, 총 15과목, 석차등급</t>
-  </si>
-  <si>
-    <t>인성(20) 학업역량(20) 전공적성(30) 발전가능성(30)</t>
-  </si>
-  <si>
-    <t>1:2 제출서류기반 개별면접, 인성(30) 전공적합성(40) 의사소통능력(30), 10분내외</t>
-  </si>
-  <si>
-    <t>해당없음</t>
-  </si>
-  <si>
-    <t>학교생활기록부</t>
-  </si>
-  <si>
-    <t>{ false}</t>
-  </si>
-  <si>
-    <t>2022 명지인재에서 분리</t>
+    <t>교과 60, 국수영과 각 교과별 상위 5과목, 점수가 높은 순으로 30:30:25:15, 석차등급</t>
+  </si>
+  <si>
+    <t>제출서류기반 지원동기(10) 자기주도적 학습능력(40) 전공적합성(30) 인성 및 사회성(20)</t>
+  </si>
+  <si>
+    <t>9.10.(금) ~ 9.14.(화) 17:00</t>
+  </si>
+  <si>
+    <t>11.26.(금)</t>
+  </si>
+  <si>
+    <t>6.2:1</t>
+  </si>
+  <si>
+    <t>5.1:1</t>
+  </si>
+  <si>
+    <t>건축공학부</t>
+  </si>
+  <si>
+    <t>3.9:1</t>
+  </si>
+  <si>
+    <t>3.4:1</t>
+  </si>
+  <si>
+    <t>4.6:1</t>
+  </si>
+  <si>
+    <t>세종대</t>
+  </si>
+  <si>
+    <t>지역균형</t>
+  </si>
+  <si>
+    <t>국내 정규 고교 졸업(예정)자로서 4개 학기 이상 학교생활기록부 성적이 있는 자 중 학교장 추천을 받은 자</t>
+  </si>
+  <si>
+    <t>교과 100, 가중치 없음, 국수영과 전과목, 석차등급</t>
   </si>
   <si>
     <t>9.10.(금) ~ 9.14.(화) 18:00</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>11.19.(금) 15:00</t>
-  </si>
-  <si>
-    <t>11.28.(일)</t>
-  </si>
-  <si>
-    <t>12.9.(목) 15:00</t>
-  </si>
-  <si>
-    <t>4.2:1</t>
-  </si>
-  <si>
-    <t>4.18:1</t>
-  </si>
-  <si>
-    <t>7.8:1</t>
-  </si>
-  <si>
-    <t>명지인재서류</t>
-  </si>
-  <si>
-    <t>일괄합산</t>
-  </si>
-  <si>
-    <t>인성(20) 학업역량(30) 전공적성(30) 발전가능성(20)</t>
-  </si>
-  <si>
-    <t>학교생활기록부, 자기소개서</t>
-  </si>
-  <si>
-    <t>{없음 true}</t>
-  </si>
-  <si>
-    <t>서울시립대</t>
-  </si>
-  <si>
-    <t>고교 졸업(예정)자 또는 동등학력 이상 인정된 자</t>
-  </si>
-  <si>
-    <t>2~4배수</t>
-  </si>
-  <si>
-    <t>1단계(60) + 면접(40)</t>
-  </si>
-  <si>
-    <t>학업역량(35) 잠재역량(40) 사회역량(25)</t>
-  </si>
-  <si>
-    <t>1:2 제출서류기반 개별면접, 학업역량(35) 잠재역량(40) 사회역량(25), 15분</t>
-  </si>
-  <si>
-    <t>{지원동기 및 진로계획 800자 true}</t>
+    <t>11.11.(목) 17:00 이후</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>5.31:1</t>
+  </si>
+  <si>
+    <t>4.86:1</t>
+  </si>
+  <si>
+    <t>4.73:1</t>
+  </si>
+  <si>
+    <t>5.63:1</t>
+  </si>
+  <si>
+    <t>학생부우수자</t>
+  </si>
+  <si>
+    <t>국내 정규 고교 졸업(예정)자로서 4개 학기 이상 학교생활기록부 성적이 있는 자</t>
+  </si>
+  <si>
+    <t>국어, 수학(미적분/기하), 영어, 과탐(1과목) 중 2개 합 6등급 이내</t>
+  </si>
+  <si>
+    <t>12.16.(목) 17:00 이후</t>
+  </si>
+  <si>
+    <t>70%컷</t>
+  </si>
+  <si>
+    <t>4.75:1</t>
+  </si>
+  <si>
+    <t>4.78:1</t>
+  </si>
+  <si>
+    <t>한양대</t>
+  </si>
+  <si>
+    <t>지역균형발전</t>
+  </si>
+  <si>
+    <t>2021년 2월 이후 국내 고교 졸업(예정)자로서 5개 학기 이상 국내 고교 성적 취득 및 출신 고등학교장의 추천을 받은 자</t>
+  </si>
+  <si>
+    <t>교과 100, 가중치 없음, 국수영사과한국사 전과목, (공통 및 일반선택) 석차등급, (진로선택) 상위 3과목, 성취도</t>
+  </si>
+  <si>
+    <t>2022 학생부교과전형 개명</t>
   </si>
   <si>
     <t>9.10.(금) ~ 9.13.(월) 18:00</t>
   </si>
   <si>
-    <t>9.14.(화) 18:00</t>
-  </si>
-  <si>
-    <t>11.19.(금)</t>
-  </si>
-  <si>
-    <t>(면접)11.27.(토)</t>
-  </si>
-  <si>
-    <t>12.16.(목)</t>
-  </si>
-  <si>
-    <t>5.88:1</t>
-  </si>
-  <si>
-    <t>6.25:1</t>
-  </si>
-  <si>
-    <t>6.13:1</t>
-  </si>
-  <si>
-    <t>성균관대</t>
-  </si>
-  <si>
-    <t>계열모집</t>
-  </si>
-  <si>
-    <t>공학계열</t>
-  </si>
-  <si>
-    <t>학업수월성(25) 학업충실성(25) 전공적합성(15) 활동다양성(15) 자기주도성(10) 발전가능성(10)</t>
-  </si>
-  <si>
-    <t>{지원동기 및 노력 800자 true}</t>
-  </si>
-  <si>
-    <t>2020부터 성균인재전형에서 명칭변경모집</t>
+    <t>10.19.(화)</t>
+  </si>
+  <si>
+    <t>5.00:1</t>
+  </si>
+  <si>
+    <t>9.67:1</t>
+  </si>
+  <si>
+    <t>7.29:1</t>
+  </si>
+  <si>
+    <t>7.00:1</t>
+  </si>
+  <si>
+    <t>6.50:1</t>
+  </si>
+  <si>
+    <t>10.00:1</t>
+  </si>
+  <si>
+    <t>한양대ERICA</t>
+  </si>
+  <si>
+    <t>학생부교과(지역균형선발)</t>
+  </si>
+  <si>
+    <t>2021년 2월 이후 국내 정규 고교 졸업(예정)자로서 통산 3개학기 이상 국내 고교 성적 취득자</t>
+  </si>
+  <si>
+    <t>교과 100, 가중치 없음, 국수영사과한국사 교과 전과목, 석차등급</t>
   </si>
   <si>
     <t>9.10.(금) ~ 9.13.(월) 17:00</t>
   </si>
   <si>
-    <t>9.14.(화) 17:00</t>
-  </si>
-  <si>
-    <t>12.16.(목) 이전</t>
-  </si>
-  <si>
-    <t>11.56:1</t>
-  </si>
-  <si>
-    <t>13.78:1</t>
-  </si>
-  <si>
-    <t>8.35:1</t>
-  </si>
-  <si>
-    <t>세종대</t>
-  </si>
-  <si>
-    <t>창의인재</t>
-  </si>
-  <si>
-    <t>디자인이노베이션전공</t>
-  </si>
-  <si>
-    <t>학업역량(30) 전공적합성(35) 창의성 및 발전가능성(20) 인성(15)</t>
-  </si>
-  <si>
-    <t>1:2 제출서류기반 개별면접, 전공적합성(40) 발전가능성(35) 의사소통능력 및 인성(25), 9분 내외</t>
-  </si>
-  <si>
-    <t>9.15.(수) 17:00</t>
-  </si>
-  <si>
-    <t>11.25.(목)</t>
-  </si>
-  <si>
-    <t>(면접)12.04.(토)</t>
-  </si>
-  <si>
-    <t>12.16.(목) 17:00 이후</t>
-  </si>
-  <si>
-    <t>70%컷</t>
-  </si>
-  <si>
-    <t>8.23:1</t>
-  </si>
-  <si>
-    <t>7.90:1</t>
-  </si>
-  <si>
-    <t>9.71:1</t>
-  </si>
-  <si>
-    <t>아주대</t>
-  </si>
-  <si>
-    <t>ACE</t>
-  </si>
-  <si>
-    <t>교통시스템공학과</t>
-  </si>
-  <si>
-    <t>학업역량(28) 목표의식(17) 자기주도성(20) 공동체의식(15) 성실성(20)</t>
-  </si>
-  <si>
-    <t>1:2 제출서류기반 개별면접, 학업역량(36) 주도성(34) 대인역량(20) 의사소통능력(10), 10분 내외</t>
-  </si>
-  <si>
-    <t>{지원동기와 학업계획 800자 true}</t>
-  </si>
-  <si>
-    <t>9.10.(금) ~ 9.14.(화) 17:00</t>
-  </si>
-  <si>
-    <t>9.24.(금) 17:00</t>
-  </si>
-  <si>
-    <t>11.16.(화)</t>
-  </si>
-  <si>
-    <t>11.21.(일)</t>
-  </si>
-  <si>
-    <t>5.2:1</t>
-  </si>
-  <si>
-    <t>5.62:1</t>
-  </si>
-  <si>
-    <t>7.07:1</t>
-  </si>
-  <si>
-    <t>미디어학과</t>
-  </si>
-  <si>
-    <t>7.98:1</t>
-  </si>
-  <si>
-    <t>7.11:1</t>
-  </si>
-  <si>
-    <t>8.04:1</t>
-  </si>
-  <si>
-    <t>다산인재</t>
-  </si>
-  <si>
-    <t>고교 졸업(예정)자 또는 동등학력 이상 인정된 자로서 다산형 인재 핵심역량(융복합 사고 역량, 실천적 창의 역량, 의사소통 역량, 글로벌 역량)에 강점이 있는 자</t>
-  </si>
-  <si>
-    <t>학업역량(30) 목표의식(20) 자기주도성(31) 공동체의식(9) 성실성(10)</t>
-  </si>
-  <si>
-    <t>5.0:1</t>
-  </si>
-  <si>
-    <t>5.25:1</t>
-  </si>
-  <si>
-    <t>5.57:1</t>
-  </si>
-  <si>
-    <t>7.38:1</t>
-  </si>
-  <si>
-    <t>10.081:1</t>
-  </si>
-  <si>
-    <t>7.50:1</t>
-  </si>
-  <si>
-    <t>한국기술교대</t>
-  </si>
-  <si>
-    <t>지역인재</t>
-  </si>
-  <si>
-    <t>디자인공학전공</t>
-  </si>
-  <si>
-    <t>고교 졸업(예정)자로서 대전-세종-충남-충북지역 소재 정규 고교에서 입학부터 졸업까지 3학년 전 과정을 이수한 자</t>
-  </si>
-  <si>
-    <t>4배수</t>
-  </si>
-  <si>
-    <t>학업역량(20), 전공적합성(20), 나우리인성(20), 발전가능성(40)</t>
-  </si>
-  <si>
-    <t>1:1 제출서류기반 개별면접, 전공적합성영역(10분 내외), 인성영역(10분 내외)</t>
-  </si>
-  <si>
-    <t>9.10.(금) ~ 9.14.(화) 19:00</t>
-  </si>
-  <si>
-    <t>11.03.(수) (예정)</t>
-  </si>
-  <si>
-    <t>(면접)11.07.(일)</t>
-  </si>
-  <si>
-    <t>11.19.(금) (예정)</t>
-  </si>
-  <si>
-    <t>5.33:1</t>
-  </si>
-  <si>
-    <t>8.86:1</t>
-  </si>
-  <si>
-    <t>12.00:1</t>
-  </si>
-  <si>
-    <t>국내 정규 고교 졸업(예정)자로서 창의적 사고와 능동적 실천능력을 갖추고 전공 분야에 대한 열정과 우수한 재능을 가진 자</t>
-  </si>
-  <si>
-    <t>(면접)11.06.(토)</t>
-  </si>
-  <si>
-    <t>4.63:1</t>
+    <t>12.15.(수)</t>
+  </si>
+  <si>
+    <t>6.75:1</t>
+  </si>
+  <si>
+    <t>5.8:1</t>
+  </si>
+  <si>
+    <t>13.71:1</t>
+  </si>
+  <si>
+    <t>홍익대</t>
+  </si>
+  <si>
+    <t>학교장추천자</t>
+  </si>
+  <si>
+    <t>2021년 2월 이후 고교 졸업(예정)자로, 국내 고교에서 3학기 이상 이수한 자, 고교별 5명 이내</t>
+  </si>
+  <si>
+    <t>국어, 수학(미적분/기하), 영어, 과탐(1과목) 중 3개 합 8등급 이내 및 한국사 4등급 이내</t>
+  </si>
+  <si>
+    <t>교과 100, 국영수과, (공통 및 일반선택)(90) 석차등급 + (진로선택)(10) 성취도</t>
+  </si>
+  <si>
+    <t>2022 교과우수자전형 개명</t>
+  </si>
+  <si>
+    <t>13.67:1</t>
+  </si>
+  <si>
+    <t>6.78:1</t>
+  </si>
+  <si>
+    <t>6.63:1</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +944,7 @@
         <v>55</v>
       </c>
       <c r="I3">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
         <v>56</v>
@@ -1031,104 +956,104 @@
         <v>58</v>
       </c>
       <c r="M3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" t="s">
         <v>59</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>60</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>61</v>
       </c>
-      <c r="P3" t="s">
-        <v>62</v>
-      </c>
       <c r="Q3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" t="s">
         <v>63</v>
       </c>
-      <c r="R3" t="s">
+      <c r="V3" t="s">
         <v>64</v>
       </c>
-      <c r="S3" t="s">
-        <v>62</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="W3" t="s">
+        <v>58</v>
+      </c>
+      <c r="X3" t="s">
         <v>65</v>
       </c>
-      <c r="U3" t="s">
+      <c r="Y3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB3" t="s">
         <v>66</v>
       </c>
-      <c r="V3" t="s">
+      <c r="AC3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD3">
+        <v>38</v>
+      </c>
+      <c r="AE3" t="s">
         <v>67</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AF3">
+        <v>51</v>
+      </c>
+      <c r="AG3">
+        <v>3.1053333</v>
+      </c>
+      <c r="AH3">
+        <v>3.9031668</v>
+      </c>
+      <c r="AI3">
+        <v>4.4013333</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>38</v>
+      </c>
+      <c r="AL3" t="s">
         <v>68</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>3.6792963</v>
+      </c>
+      <c r="AP3">
+        <v>2.954</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>37</v>
+      </c>
+      <c r="AS3" t="s">
         <v>69</v>
       </c>
-      <c r="Y3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD3">
-        <v>11</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF3">
-        <v>11</v>
-      </c>
-      <c r="AG3">
-        <v>3.68</v>
-      </c>
-      <c r="AH3">
-        <v>4.1</v>
-      </c>
-      <c r="AI3">
-        <v>4.58</v>
-      </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <v>11</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
-        <v>0</v>
-      </c>
-      <c r="AO3">
-        <v>4.03</v>
-      </c>
-      <c r="AP3">
-        <v>4.85</v>
-      </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3">
-        <v>10</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>76</v>
-      </c>
       <c r="AT3">
         <v>0</v>
       </c>
@@ -1136,10 +1061,10 @@
         <v>0</v>
       </c>
       <c r="AV3">
-        <v>3.88</v>
+        <v>3.8772316</v>
       </c>
       <c r="AW3">
-        <v>4.56</v>
+        <v>4.327</v>
       </c>
       <c r="AX3">
         <v>0</v>
@@ -1159,7 +1084,7 @@
         <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
         <v>53</v>
@@ -1171,94 +1096,94 @@
         <v>55</v>
       </c>
       <c r="I4">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="K4" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="L4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="M4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" t="s">
         <v>61</v>
       </c>
-      <c r="P4" t="s">
-        <v>62</v>
-      </c>
       <c r="Q4" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="R4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" t="s">
+        <v>62</v>
+      </c>
+      <c r="U4" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" t="s">
+        <v>58</v>
+      </c>
+      <c r="X4" t="s">
         <v>65</v>
       </c>
-      <c r="S4" t="s">
-        <v>62</v>
-      </c>
-      <c r="T4" t="s">
-        <v>65</v>
-      </c>
-      <c r="U4" t="s">
-        <v>80</v>
-      </c>
-      <c r="V4" t="s">
-        <v>81</v>
-      </c>
-      <c r="W4" t="s">
-        <v>68</v>
-      </c>
-      <c r="X4" t="s">
-        <v>69</v>
-      </c>
       <c r="Y4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="Z4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AA4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AB4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="AC4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AD4">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="AE4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AF4">
         <v>11</v>
       </c>
       <c r="AG4">
-        <v>3.68</v>
+        <v>3.437</v>
       </c>
       <c r="AH4">
-        <v>4.1</v>
+        <v>3.9651449</v>
       </c>
       <c r="AI4">
-        <v>4.58</v>
+        <v>4.54</v>
       </c>
       <c r="AJ4">
         <v>0</v>
       </c>
       <c r="AK4">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="AL4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AM4">
         <v>0</v>
@@ -1267,19 +1192,19 @@
         <v>0</v>
       </c>
       <c r="AO4">
-        <v>4.03</v>
+        <v>3.9573889</v>
       </c>
       <c r="AP4">
-        <v>4.85</v>
+        <v>4.458667</v>
       </c>
       <c r="AQ4">
         <v>0</v>
       </c>
       <c r="AR4">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="AS4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AT4">
         <v>0</v>
@@ -1288,10 +1213,10 @@
         <v>0</v>
       </c>
       <c r="AV4">
-        <v>3.88</v>
+        <v>4.232037</v>
       </c>
       <c r="AW4">
-        <v>4.56</v>
+        <v>5.4</v>
       </c>
       <c r="AX4">
         <v>0</v>
@@ -1302,7 +1227,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
         <v>50</v>
@@ -1311,10 +1236,10 @@
         <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
         <v>54</v>
@@ -1323,10 +1248,10 @@
         <v>55</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="K5" t="s">
         <v>57</v>
@@ -1335,103 +1260,103 @@
         <v>58</v>
       </c>
       <c r="M5" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O5" t="s">
+        <v>80</v>
+      </c>
+      <c r="P5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>82</v>
+      </c>
+      <c r="R5" t="s">
+        <v>62</v>
+      </c>
+      <c r="S5" t="s">
+        <v>81</v>
+      </c>
+      <c r="T5" t="s">
+        <v>62</v>
+      </c>
+      <c r="U5" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W5" t="s">
+        <v>58</v>
+      </c>
+      <c r="X5" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB5" t="s">
         <v>84</v>
       </c>
-      <c r="N5" t="s">
+      <c r="AC5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5">
+        <v>12</v>
+      </c>
+      <c r="AE5" t="s">
         <v>85</v>
       </c>
-      <c r="O5" t="s">
-        <v>61</v>
-      </c>
-      <c r="P5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="AF5">
+        <v>21</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>2.64</v>
+      </c>
+      <c r="AI5">
+        <v>3.5</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>12</v>
+      </c>
+      <c r="AL5" t="s">
         <v>86</v>
       </c>
-      <c r="R5" t="s">
-        <v>87</v>
-      </c>
-      <c r="S5" t="s">
-        <v>62</v>
-      </c>
-      <c r="T5" t="s">
-        <v>65</v>
-      </c>
-      <c r="U5" t="s">
-        <v>80</v>
-      </c>
-      <c r="V5" t="s">
-        <v>88</v>
-      </c>
-      <c r="W5" t="s">
-        <v>70</v>
-      </c>
-      <c r="X5" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD5">
-        <v>8</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
-      <c r="AG5">
-        <v>0</v>
-      </c>
-      <c r="AH5">
-        <v>2.32</v>
-      </c>
-      <c r="AI5">
-        <v>0</v>
-      </c>
-      <c r="AJ5">
-        <v>0</v>
-      </c>
-      <c r="AK5">
-        <v>8</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>95</v>
-      </c>
       <c r="AM5">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AN5">
         <v>0</v>
       </c>
       <c r="AO5">
-        <v>3.07</v>
+        <v>2.87</v>
       </c>
       <c r="AP5">
-        <v>0</v>
+        <v>3.36</v>
       </c>
       <c r="AQ5">
         <v>0</v>
       </c>
       <c r="AR5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="AS5" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="AT5">
         <v>0</v>
@@ -1440,10 +1365,10 @@
         <v>0</v>
       </c>
       <c r="AV5">
-        <v>2.9</v>
+        <v>2.95</v>
       </c>
       <c r="AW5">
-        <v>0</v>
+        <v>4.05</v>
       </c>
       <c r="AX5">
         <v>0</v>
@@ -1454,7 +1379,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
         <v>50</v>
@@ -1463,10 +1388,10 @@
         <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
         <v>54</v>
@@ -1475,115 +1400,115 @@
         <v>55</v>
       </c>
       <c r="I6">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="J6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" t="s">
+        <v>58</v>
+      </c>
+      <c r="N6" t="s">
+        <v>79</v>
+      </c>
+      <c r="O6" t="s">
+        <v>80</v>
+      </c>
+      <c r="P6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>82</v>
+      </c>
+      <c r="R6" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" t="s">
+        <v>81</v>
+      </c>
+      <c r="T6" t="s">
+        <v>62</v>
+      </c>
+      <c r="U6" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" t="s">
+        <v>64</v>
+      </c>
+      <c r="W6" t="s">
+        <v>58</v>
+      </c>
+      <c r="X6" t="s">
         <v>83</v>
       </c>
-      <c r="K6" t="s">
-        <v>78</v>
-      </c>
-      <c r="L6" t="s">
-        <v>70</v>
-      </c>
-      <c r="M6" t="s">
-        <v>70</v>
-      </c>
-      <c r="N6" t="s">
-        <v>58</v>
-      </c>
-      <c r="O6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>100</v>
-      </c>
-      <c r="R6" t="s">
-        <v>65</v>
-      </c>
-      <c r="S6" t="s">
-        <v>62</v>
-      </c>
-      <c r="T6" t="s">
-        <v>65</v>
-      </c>
-      <c r="U6" t="s">
-        <v>80</v>
-      </c>
-      <c r="V6" t="s">
-        <v>101</v>
-      </c>
-      <c r="W6" t="s">
-        <v>102</v>
-      </c>
-      <c r="X6" t="s">
-        <v>103</v>
-      </c>
       <c r="Y6" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="Z6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AA6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AB6" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="AC6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AD6">
-        <v>230</v>
+        <v>14</v>
       </c>
       <c r="AE6" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="AF6">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AG6">
         <v>0</v>
       </c>
       <c r="AH6">
-        <v>0</v>
+        <v>2.3</v>
       </c>
       <c r="AI6">
-        <v>0</v>
+        <v>3.22</v>
       </c>
       <c r="AJ6">
         <v>0</v>
       </c>
       <c r="AK6">
-        <v>223</v>
+        <v>14</v>
       </c>
       <c r="AL6" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="AM6">
-        <v>728</v>
+        <v>19</v>
       </c>
       <c r="AN6">
         <v>0</v>
       </c>
       <c r="AO6">
-        <v>0</v>
+        <v>2.26</v>
       </c>
       <c r="AP6">
-        <v>0</v>
+        <v>2.82</v>
       </c>
       <c r="AQ6">
         <v>0</v>
       </c>
       <c r="AR6">
-        <v>267</v>
+        <v>14</v>
       </c>
       <c r="AS6" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="AT6">
         <v>0</v>
@@ -1592,10 +1517,10 @@
         <v>0</v>
       </c>
       <c r="AV6">
-        <v>0</v>
+        <v>2.31</v>
       </c>
       <c r="AW6">
-        <v>0</v>
+        <v>2.83</v>
       </c>
       <c r="AX6">
         <v>0</v>
@@ -1606,7 +1531,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
         <v>50</v>
@@ -1615,10 +1540,10 @@
         <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="G7" t="s">
         <v>54</v>
@@ -1627,10 +1552,10 @@
         <v>55</v>
       </c>
       <c r="I7">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="K7" t="s">
         <v>57</v>
@@ -1639,82 +1564,82 @@
         <v>58</v>
       </c>
       <c r="M7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" t="s">
         <v>59</v>
       </c>
-      <c r="N7" t="s">
-        <v>60</v>
-      </c>
       <c r="O7" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="P7" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="Q7" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="R7" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="S7" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="T7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U7" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="V7" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="W7" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="X7" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="Y7" t="s">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="Z7" t="s">
-        <v>115</v>
+        <v>58</v>
       </c>
       <c r="AA7" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="AB7" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="AC7" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="AD7">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="AE7" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="AF7">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AG7">
         <v>0</v>
       </c>
       <c r="AH7">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="AI7">
-        <v>2.91</v>
+        <v>0</v>
       </c>
       <c r="AJ7">
         <v>0</v>
       </c>
       <c r="AK7">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="AL7" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="AM7">
         <v>0</v>
@@ -1723,19 +1648,19 @@
         <v>0</v>
       </c>
       <c r="AO7">
-        <v>2.8</v>
+        <v>2.21</v>
       </c>
       <c r="AP7">
-        <v>3.35</v>
+        <v>2.27</v>
       </c>
       <c r="AQ7">
         <v>0</v>
       </c>
       <c r="AR7">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="AS7" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="AT7">
         <v>0</v>
@@ -1744,10 +1669,10 @@
         <v>0</v>
       </c>
       <c r="AV7">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="AW7">
-        <v>3.18</v>
+        <v>0</v>
       </c>
       <c r="AX7">
         <v>0</v>
@@ -1758,7 +1683,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>50</v>
@@ -1767,10 +1692,10 @@
         <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
@@ -1779,10 +1704,10 @@
         <v>55</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="K8" t="s">
         <v>57</v>
@@ -1791,82 +1716,82 @@
         <v>58</v>
       </c>
       <c r="M8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" t="s">
         <v>59</v>
       </c>
-      <c r="N8" t="s">
-        <v>60</v>
-      </c>
       <c r="O8" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="P8" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="Q8" t="s">
-        <v>125</v>
+        <v>62</v>
       </c>
       <c r="R8" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="S8" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="T8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U8" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="V8" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="W8" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="X8" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="Y8" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="Z8" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="AA8" t="s">
-        <v>131</v>
+        <v>58</v>
       </c>
       <c r="AB8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AC8" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AD8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="AF8">
         <v>0</v>
       </c>
       <c r="AG8">
-        <v>2.61</v>
+        <v>0</v>
       </c>
       <c r="AH8">
-        <v>3.05</v>
+        <v>0</v>
       </c>
       <c r="AI8">
-        <v>3.78</v>
+        <v>0</v>
       </c>
       <c r="AJ8">
         <v>0</v>
       </c>
       <c r="AK8">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="AL8" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="AM8">
         <v>0</v>
@@ -1875,19 +1800,19 @@
         <v>0</v>
       </c>
       <c r="AO8">
-        <v>3.4</v>
+        <v>2.19</v>
       </c>
       <c r="AP8">
-        <v>6.03</v>
+        <v>2.37</v>
       </c>
       <c r="AQ8">
         <v>0</v>
       </c>
       <c r="AR8">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="AS8" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="AT8">
         <v>0</v>
@@ -1896,10 +1821,10 @@
         <v>0</v>
       </c>
       <c r="AV8">
-        <v>3.43</v>
+        <v>2.17</v>
       </c>
       <c r="AW8">
-        <v>5.31</v>
+        <v>0</v>
       </c>
       <c r="AX8">
         <v>0</v>
@@ -1910,7 +1835,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>50</v>
@@ -1919,10 +1844,10 @@
         <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="F9" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="G9" t="s">
         <v>54</v>
@@ -1931,10 +1856,10 @@
         <v>55</v>
       </c>
       <c r="I9">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K9" t="s">
         <v>57</v>
@@ -1943,82 +1868,82 @@
         <v>58</v>
       </c>
       <c r="M9" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9" t="s">
         <v>59</v>
       </c>
-      <c r="N9" t="s">
-        <v>60</v>
-      </c>
       <c r="O9" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="P9" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="Q9" t="s">
-        <v>125</v>
+        <v>62</v>
       </c>
       <c r="R9" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="S9" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="T9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U9" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="V9" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="W9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="X9" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="Y9" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="Z9" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="AA9" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="AB9" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="AC9" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="AD9">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="AE9" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="AF9">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="AG9">
-        <v>2.33</v>
+        <v>0</v>
       </c>
       <c r="AH9">
-        <v>3.33</v>
+        <v>2.27</v>
       </c>
       <c r="AI9">
-        <v>6.26</v>
+        <v>2.41</v>
       </c>
       <c r="AJ9">
         <v>0</v>
       </c>
       <c r="AK9">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="AL9" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="AM9">
         <v>0</v>
@@ -2027,19 +1952,19 @@
         <v>0</v>
       </c>
       <c r="AO9">
-        <v>3.18</v>
+        <v>2.21</v>
       </c>
       <c r="AP9">
-        <v>6.58</v>
+        <v>2.27</v>
       </c>
       <c r="AQ9">
         <v>0</v>
       </c>
       <c r="AR9">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="AS9" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="AT9">
         <v>0</v>
@@ -2048,10 +1973,10 @@
         <v>0</v>
       </c>
       <c r="AV9">
-        <v>3.16</v>
+        <v>2.4</v>
       </c>
       <c r="AW9">
-        <v>6.03</v>
+        <v>0</v>
       </c>
       <c r="AX9">
         <v>0</v>
@@ -2062,7 +1987,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
         <v>50</v>
@@ -2071,10 +1996,10 @@
         <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="F10" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
         <v>54</v>
@@ -2083,94 +2008,94 @@
         <v>55</v>
       </c>
       <c r="I10">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="J10" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="K10" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="L10" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="M10" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O10" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="P10" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="Q10" t="s">
-        <v>141</v>
+        <v>62</v>
       </c>
       <c r="R10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S10" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="T10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U10" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="V10" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="W10" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="X10" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="Y10" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="Z10" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AA10" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AB10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="AC10" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="AD10">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="AE10" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="AF10">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="AG10">
-        <v>2.76</v>
+        <v>0</v>
       </c>
       <c r="AH10">
-        <v>3.56</v>
+        <v>2.37</v>
       </c>
       <c r="AI10">
-        <v>4.71</v>
+        <v>2.54</v>
       </c>
       <c r="AJ10">
         <v>0</v>
       </c>
       <c r="AK10">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="AL10" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="AM10">
         <v>0</v>
@@ -2179,19 +2104,19 @@
         <v>0</v>
       </c>
       <c r="AO10">
-        <v>3.4</v>
+        <v>2.19</v>
       </c>
       <c r="AP10">
-        <v>4.23</v>
+        <v>2.37</v>
       </c>
       <c r="AQ10">
         <v>0</v>
       </c>
       <c r="AR10">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="AS10" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="AT10">
         <v>0</v>
@@ -2200,10 +2125,10 @@
         <v>0</v>
       </c>
       <c r="AV10">
-        <v>3.37</v>
+        <v>2.17</v>
       </c>
       <c r="AW10">
-        <v>3.97</v>
+        <v>0</v>
       </c>
       <c r="AX10">
         <v>0</v>
@@ -2214,7 +2139,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
         <v>50</v>
@@ -2223,10 +2148,10 @@
         <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="F11" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
         <v>54</v>
@@ -2235,94 +2160,94 @@
         <v>55</v>
       </c>
       <c r="I11">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="J11" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="K11" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="L11" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="M11" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O11" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="P11" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="Q11" t="s">
-        <v>141</v>
+        <v>62</v>
       </c>
       <c r="R11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S11" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="T11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U11" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="V11" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="W11" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="X11" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="Y11" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="Z11" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AA11" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AB11" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="AC11" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="AD11">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="AE11" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="AF11">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AG11">
-        <v>2.69</v>
+        <v>0</v>
       </c>
       <c r="AH11">
-        <v>4.2</v>
+        <v>1.33</v>
       </c>
       <c r="AI11">
-        <v>7.48</v>
+        <v>1.48</v>
       </c>
       <c r="AJ11">
         <v>0</v>
       </c>
       <c r="AK11">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="AL11" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="AM11">
         <v>0</v>
@@ -2331,19 +2256,19 @@
         <v>0</v>
       </c>
       <c r="AO11">
-        <v>3.36</v>
+        <v>1.34</v>
       </c>
       <c r="AP11">
-        <v>4.42</v>
+        <v>0</v>
       </c>
       <c r="AQ11">
         <v>0</v>
       </c>
       <c r="AR11">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AS11" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="AT11">
         <v>0</v>
@@ -2352,10 +2277,10 @@
         <v>0</v>
       </c>
       <c r="AV11">
-        <v>3.95</v>
+        <v>1.23</v>
       </c>
       <c r="AW11">
-        <v>5.77</v>
+        <v>0</v>
       </c>
       <c r="AX11">
         <v>0</v>
@@ -2366,7 +2291,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
         <v>50</v>
@@ -2375,10 +2300,10 @@
         <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>110</v>
       </c>
       <c r="F12" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
         <v>54</v>
@@ -2387,10 +2312,10 @@
         <v>55</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J12" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="K12" t="s">
         <v>57</v>
@@ -2399,82 +2324,82 @@
         <v>58</v>
       </c>
       <c r="M12" t="s">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="N12" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="O12" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="P12" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="Q12" t="s">
-        <v>153</v>
+        <v>62</v>
       </c>
       <c r="R12" t="s">
-        <v>154</v>
+        <v>62</v>
       </c>
       <c r="S12" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="T12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="V12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="W12" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="X12" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="Y12" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="Z12" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="AA12" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="AB12" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="AC12" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="AD12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE12" t="s">
-        <v>159</v>
+        <v>119</v>
       </c>
       <c r="AF12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="AG12">
         <v>0</v>
       </c>
       <c r="AH12">
-        <v>4.25</v>
+        <v>1.33</v>
       </c>
       <c r="AI12">
-        <v>0</v>
+        <v>1.39</v>
       </c>
       <c r="AJ12">
         <v>0</v>
       </c>
       <c r="AK12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AL12" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="AM12">
         <v>0</v>
@@ -2483,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="AO12">
-        <v>4.16</v>
+        <v>1.38</v>
       </c>
       <c r="AP12">
         <v>0</v>
@@ -2492,10 +2417,10 @@
         <v>0</v>
       </c>
       <c r="AR12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AS12" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="AT12">
         <v>0</v>
@@ -2504,7 +2429,7 @@
         <v>0</v>
       </c>
       <c r="AV12">
-        <v>4.37</v>
+        <v>1.23</v>
       </c>
       <c r="AW12">
         <v>0</v>
@@ -2518,7 +2443,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -2527,10 +2452,10 @@
         <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>150</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s">
         <v>54</v>
@@ -2539,10 +2464,10 @@
         <v>55</v>
       </c>
       <c r="I13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J13" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="K13" t="s">
         <v>57</v>
@@ -2551,70 +2476,70 @@
         <v>58</v>
       </c>
       <c r="M13" t="s">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="N13" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="O13" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="P13" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="Q13" t="s">
-        <v>153</v>
+        <v>62</v>
       </c>
       <c r="R13" t="s">
-        <v>154</v>
+        <v>62</v>
       </c>
       <c r="S13" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="T13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="U13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="V13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="W13" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="X13" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="Y13" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="Z13" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="AA13" t="s">
-        <v>163</v>
+        <v>58</v>
       </c>
       <c r="AB13" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="AC13" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AD13">
         <v>8</v>
       </c>
       <c r="AE13" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="AF13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG13">
         <v>0</v>
       </c>
       <c r="AH13">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="AI13">
         <v>0</v>
@@ -2623,31 +2548,31 @@
         <v>0</v>
       </c>
       <c r="AK13">
+        <v>8</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>2.58</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13">
         <v>7</v>
       </c>
-      <c r="AL13" t="s">
-        <v>160</v>
-      </c>
-      <c r="AM13">
-        <v>0</v>
-      </c>
-      <c r="AN13">
-        <v>0</v>
-      </c>
-      <c r="AO13">
-        <v>4.16</v>
-      </c>
-      <c r="AP13">
-        <v>0</v>
-      </c>
-      <c r="AQ13">
-        <v>0</v>
-      </c>
-      <c r="AR13">
-        <v>6</v>
-      </c>
       <c r="AS13" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="AT13">
         <v>0</v>
@@ -2656,12 +2581,164 @@
         <v>0</v>
       </c>
       <c r="AV13">
-        <v>4.37</v>
+        <v>2.41</v>
       </c>
       <c r="AW13">
         <v>0</v>
       </c>
       <c r="AX13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>133</v>
+      </c>
+      <c r="K14" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" t="s">
+        <v>58</v>
+      </c>
+      <c r="N14" t="s">
+        <v>59</v>
+      </c>
+      <c r="O14" t="s">
+        <v>134</v>
+      </c>
+      <c r="P14" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R14" t="s">
+        <v>62</v>
+      </c>
+      <c r="S14" t="s">
+        <v>135</v>
+      </c>
+      <c r="T14" t="s">
+        <v>62</v>
+      </c>
+      <c r="U14" t="s">
+        <v>63</v>
+      </c>
+      <c r="V14" t="s">
+        <v>64</v>
+      </c>
+      <c r="W14" t="s">
+        <v>136</v>
+      </c>
+      <c r="X14" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD14">
+        <v>9</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF14">
+        <v>9</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <v>2.37</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>9</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <v>2.63</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
+      <c r="AR14">
+        <v>35</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AT14">
+        <v>0</v>
+      </c>
+      <c r="AU14">
+        <v>0</v>
+      </c>
+      <c r="AV14">
+        <v>0</v>
+      </c>
+      <c r="AW14">
+        <v>0</v>
+      </c>
+      <c r="AX14">
         <v>0</v>
       </c>
     </row>

</xml_diff>